<commit_message>
add more feature to project
</commit_message>
<xml_diff>
--- a/testcases/Facebook.xlsx
+++ b/testcases/Facebook.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="POM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,30 +25,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>Test Id</t>
+  </si>
+  <si>
+    <t>Test_01</t>
+  </si>
+  <si>
+    <t>Test_02</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
+    <t>Object Type</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>GO_URL</t>
+  </si>
+  <si>
+    <t>SET_TEXT</t>
+  </si>
+  <si>
+    <t>CLICK</t>
+  </si>
+  <si>
+    <t>passw0rd</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>login.email</t>
+  </si>
+  <si>
+    <t>login.password</t>
+  </si>
+  <si>
+    <t>login.btnLogin</t>
+  </si>
+  <si>
+    <t>login.url</t>
+  </si>
+  <si>
+    <t>SCREEN_SHOT</t>
+  </si>
+  <si>
+    <t>screenshots/screen.jpg</t>
+  </si>
   <si>
     <t>User Name</t>
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>Test Id</t>
-  </si>
-  <si>
-    <t>Test_01</t>
-  </si>
-  <si>
-    <t>Test_02</t>
   </si>
 </sst>
 </file>
@@ -85,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -108,20 +157,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -396,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,43 +510,237 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="https://en-gb.facebook.com/"/>
+    <hyperlink ref="E9" r:id="rId2" display="https://en-gb.facebook.com/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>